<commit_message>
Update mining pool stats
</commit_message>
<xml_diff>
--- a/Data/updated-miner-to-region-mix.xlsx
+++ b/Data/updated-miner-to-region-mix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clair\CCAF\Week50 0905-0909\CCAF ETH PoW mining\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76F34DD-8303-4143-96CC-544F75A62EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6938F8-57A6-442C-9E69-67B658061ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C60EC255-1E12-4285-8A55-CB31130E2004}"/>
   </bookViews>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A77835-8864-4430-BA97-58A8DE1BF4F6}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1359,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>78</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1854,10 +1854,10 @@
         <v>32</v>
       </c>
       <c r="B35" s="1">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="C35" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D35" s="1">
         <v>36.9</v>
@@ -1872,7 +1872,7 @@
         <v>0.8</v>
       </c>
       <c r="H35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
@@ -1884,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>57</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>58</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>59</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="57" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>61</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>66</v>
       </c>

</xml_diff>